<commit_message>
revision sent to stefan and sascha
</commit_message>
<xml_diff>
--- a/Literature_overview_all_Stand08_07_2024.xlsx
+++ b/Literature_overview_all_Stand08_07_2024.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF87299-A6AE-4B1C-987C-FBDDBE443F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE51B651-31C2-49ED-A206-0A2F2319D12E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="15" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -8042,10 +8042,10 @@
   <dimension ref="A1:CK93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H64" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="K70" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O40" sqref="O40"/>
+      <selection pane="bottomRight" activeCell="R72" sqref="R72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>